<commit_message>
Determine whether a gene is expressed using expression counts data, not COSOPT's MeanExpLev
Using MeanExpLev deflated the number of genes considered to be expressed,
since only genes with COSOPT results would have a value for MeanExpLev.

Compress Expression-and-COSOPT-Summary.txt to fit GitHub's limits.
</commit_message>
<xml_diff>
--- a/rhythmic-and-expressed-summary.xlsx
+++ b/rhythmic-and-expressed-summary.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfc/git.repos/sunflower-rhythms-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C276BC83-D50D-D24A-8C85-183C1E17D722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35580A40-693F-F947-98F9-B1F42670EAFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{342B5EE8-23C1-DF43-9F84-7A78E71FE71B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,7 +430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B93AC8-48FC-8340-B623-80F125490AD1}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -455,14 +457,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>22328</v>
+        <v>22333</v>
       </c>
       <c r="C2" s="1">
-        <v>30166</v>
+        <v>35205</v>
       </c>
       <c r="D2" s="2">
         <f>B2/C2</f>
-        <v>0.74017105350394485</v>
+        <v>0.63437011788098285</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -470,14 +472,14 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>22374</v>
+        <v>22383</v>
       </c>
       <c r="C3" s="1">
-        <v>29950</v>
+        <v>35299</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D8" si="0">B3/C3</f>
-        <v>0.74704507512520868</v>
+        <v>0.63409728320915604</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -485,14 +487,14 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>25607</v>
+        <v>25661</v>
       </c>
       <c r="C4" s="1">
-        <v>33188</v>
+        <v>35491</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>0.77157406291430641</v>
+        <v>0.72302837339043702</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -500,14 +502,14 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>19095</v>
+        <v>19100</v>
       </c>
       <c r="C5" s="1">
-        <v>26928</v>
+        <v>35013</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0.70911319073083778</v>
+        <v>0.54551166709507892</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -515,14 +517,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>24574</v>
+        <v>24568</v>
       </c>
       <c r="C6" s="1">
-        <v>30844</v>
+        <v>35239</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>0.79671897289586302</v>
+        <v>0.69718209937852949</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -530,14 +532,14 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>26486</v>
+        <v>26490</v>
       </c>
       <c r="C7" s="1">
-        <v>33488</v>
+        <v>35492</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" ref="D7" si="1">B7/C7</f>
-        <v>0.79091017677974196</v>
+        <v>0.74636537811337766</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -545,14 +547,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>19062</v>
+        <v>19064</v>
       </c>
       <c r="C8" s="1">
-        <v>26641</v>
+        <v>35005</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>0.7155136819188469</v>
+        <v>0.54460791315526358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>